<commit_message>
User will be delete, if there are no lendings
</commit_message>
<xml_diff>
--- a/public/table/barcode.xlsx
+++ b/public/table/barcode.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="767">
   <si>
     <t xml:space="preserve">Artikel</t>
   </si>
@@ -2312,6 +2312,15 @@
   </si>
   <si>
     <t xml:space="preserve">Zucker für den Kaffee über der Kaffemaschine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfeffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN SH TEST 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfeffer gibts mim labor nicht</t>
   </si>
 </sst>
 </file>
@@ -2633,10 +2642,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N461"/>
+  <dimension ref="A1:N462"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A441" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C461" activeCellId="0" sqref="C461"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A452" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C462" activeCellId="0" sqref="C462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14641,6 +14650,17 @@
         <v>763</v>
       </c>
     </row>
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="B462" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="C462" s="0" t="s">
+        <v>766</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>